<commit_message>
Update Output ALL Sheet Excel
</commit_message>
<xml_diff>
--- a/thisinh.xlsx
+++ b/thisinh.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="36">
   <si>
     <t/>
   </si>
@@ -71,13 +71,16 @@
     <t>Khối B</t>
   </si>
   <si>
-    <t>8484</t>
-  </si>
-  <si>
-    <t>Minh</t>
-  </si>
-  <si>
-    <t>Hà Giang</t>
+    <t>34294</t>
+  </si>
+  <si>
+    <t>Quân</t>
+  </si>
+  <si>
+    <t>Cao Bằng</t>
+  </si>
+  <si>
+    <t>Khối C</t>
   </si>
   <si>
     <t>93202</t>
@@ -86,15 +89,18 @@
     <t>Tùng</t>
   </si>
   <si>
+    <t>Thái Bình</t>
+  </si>
+  <si>
+    <t>201901</t>
+  </si>
+  <si>
+    <t>Manh</t>
+  </si>
+  <si>
     <t>Hà Nội</t>
   </si>
   <si>
-    <t>201901</t>
-  </si>
-  <si>
-    <t>Manh</t>
-  </si>
-  <si>
     <t>Thương bệnh binh (2 điểm)</t>
   </si>
   <si>
@@ -110,22 +116,7 @@
     <t>Khu vực nông thôn (0.5 điểm)</t>
   </si>
   <si>
-    <t>Khối C</t>
-  </si>
-  <si>
     <t>100.0%</t>
-  </si>
-  <si>
-    <t>Tổng số: 3</t>
-  </si>
-  <si>
-    <t>50.0%</t>
-  </si>
-  <si>
-    <t>Tổng số: 1</t>
-  </si>
-  <si>
-    <t>16.666668%</t>
   </si>
   <si>
     <t>Tổng số: 2</t>
@@ -261,10 +252,10 @@
         <v>20</v>
       </c>
       <c r="E7" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="F7" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8">
@@ -272,13 +263,13 @@
         <v>4.0</v>
       </c>
       <c r="B8" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C8" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D8" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E8" t="s">
         <v>16</v>
@@ -292,16 +283,16 @@
         <v>5.0</v>
       </c>
       <c r="B9" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D9" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="E9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="F9" t="s">
         <v>17</v>
@@ -312,24 +303,24 @@
         <v>6.0</v>
       </c>
       <c r="B10" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C10" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D10" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E10" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F10" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12">
       <c r="F12" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -339,7 +330,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A3:G9"/>
+  <dimension ref="A3:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -347,7 +338,7 @@
   <sheetData>
     <row r="3">
       <c r="C3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4">
@@ -395,44 +386,24 @@
         <v>2.0</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C6" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="D6" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="E6" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="F6" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="B7" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D7" t="s">
-        <v>23</v>
-      </c>
-      <c r="E7" t="s">
-        <v>16</v>
-      </c>
-      <c r="F7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="F9" t="s">
-        <v>34</v>
+    <row r="8">
+      <c r="F8" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -450,7 +421,7 @@
   <sheetData>
     <row r="3">
       <c r="C3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4">
@@ -498,16 +469,16 @@
         <v>2.0</v>
       </c>
       <c r="B6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C6" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D6" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="E6" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="F6" t="s">
         <v>17</v>
@@ -515,7 +486,7 @@
     </row>
     <row r="8">
       <c r="F8" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -525,7 +496,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A3:G7"/>
+  <dimension ref="A3:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -533,7 +504,7 @@
   <sheetData>
     <row r="3">
       <c r="C3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4">
@@ -561,24 +532,44 @@
         <v>1.0</v>
       </c>
       <c r="B5" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="C5" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="D5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B6" t="s">
         <v>29</v>
       </c>
-      <c r="E5" t="s">
+      <c r="C6" t="s">
         <v>30</v>
       </c>
-      <c r="F5" t="s">
+      <c r="D6" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="7">
-      <c r="F7" t="s">
-        <v>36</v>
+      <c r="E6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="F8" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>